<commit_message>
se trae de vuelta input
</commit_message>
<xml_diff>
--- a/entidades/entidades.xlsx
+++ b/entidades/entidades.xlsx
@@ -11,7 +11,7 @@
     <sheet name="28_10_2024" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">28_10_2024!$A$1:$G$86</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">28_10_2024!$A$1:$I$86</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="514">
   <si>
     <t xml:space="preserve">entidad</t>
   </si>
@@ -34,6 +34,30 @@
     <t xml:space="preserve">sector</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">s_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">description</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">description</t>
+  </si>
+  <si>
     <t xml:space="preserve">mision</t>
   </si>
   <si>
@@ -55,6 +79,12 @@
     <t xml:space="preserve">Ambiente</t>
   </si>
   <si>
+    <t xml:space="preserve"> Encargado de la protección ambiental, la sostenibilidad y la mitigación del cambio climático en la ciudad.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entidad que lidera la gestión de riesgos y la respuesta ante emergencias en Bogotá.</t>
+  </si>
+  <si>
     <t xml:space="preserve">El IDIGER emprende acciones y genera lineamientos para la gestión del riesgo de desastres y la adaptación al cambio climático, en el marco de la coordinación del SDGR-CC en el Distrito Capital, con el fin de proteger a las personas en situación de riesgo y lograr el desarrollo sostenible de Bogotá D.C</t>
   </si>
   <si>
@@ -70,6 +100,9 @@
     <t xml:space="preserve">e739d624-2335-4c9f-87af-db9ba828e296</t>
   </si>
   <si>
+    <t xml:space="preserve">Entidad dedicada a la protección y bienestar de los animales en Bogotá.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Somos la primera entidad pública encargada de la protección y el bienestar animal, garantes de la vida de la Fauna en el Distrito Capital a través, de la formulación, implementación, seguimiento y evaluación de políticas públicas sectoriales e intersectoriales..</t>
   </si>
   <si>
@@ -85,6 +118,9 @@
     <t xml:space="preserve">eb0a045e-2518-4482-a623-8351a9340e2a</t>
   </si>
   <si>
+    <t xml:space="preserve">Jardín botánico que promueve la conservación y el estudio de la biodiversidad.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Investigar y conservar la flora de los ecosistemas altoandinos y de páramo y gestionar las coberturas vegetales urbanas, contribuyendo a la generación, aplicación y apropiación social del conocimiento para la adaptación al cambio climático, al mejoramiento de la calidad de vida y al desarrollo sostenible en el Distrito Capital y la Región</t>
   </si>
   <si>
@@ -100,6 +136,9 @@
     <t xml:space="preserve">f44cbd7c-171d-4b35-9133-8901fb67c3a0</t>
   </si>
   <si>
+    <t xml:space="preserve">Entidad que lidera la gestión ambiental y la protección de los recursos naturales.</t>
+  </si>
+  <si>
     <t xml:space="preserve">La Secretaria Distrital de Ambiente, como autoridad ambiental del Distrito Capital propende por el desarrollo sostenible de la ciudad, formulando promoviendo y orientando políticas, planes y programas que permitan la conservación, protección y recuperación del ambiente y de los bienes y servicios naturales de la Estructura Ecológica Principal y de las áreas de interés ambiental; para mejorar su calidad de vida, la relación entre la población y el entorno natural, el disfrute de los derechos fundamentales y colectivos del ambiente, respondiendo a las acciones encaminadas a  la adaptación y mitigación al cambio climático, reverdeciendo a Bogotá y promoviendo la participación de la ciudadanía en todas sus dimensiones y el cambio de los hábitos de vida.</t>
   </si>
   <si>
@@ -118,6 +157,12 @@
     <t xml:space="preserve">Cultura Recreación y Deporte</t>
   </si>
   <si>
+    <t xml:space="preserve"> Promueve el patrimonio cultural, la expresión artística, el deporte y las actividades recreativas.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medio de comunicación público encargado de informar y educar a la ciudadanía.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Capital es el Sistema de comunicación pública de Bogotá región que ubica a la ciudadanía en el centro de su operación y, mediante la inteligencia colectiva, aporta a la construcción de una sociedad participativa e incluyente, a través de la producción y circulación de contenidos informativos, culturales y educativos en múltiples plataformas y del desarrollo de estrategias de comunicación relevantes para los grupos de interés.</t>
   </si>
   <si>
@@ -133,6 +178,9 @@
     <t xml:space="preserve">9a322050-1f3a-4431-87f4-5d24fb1adcf5</t>
   </si>
   <si>
+    <t xml:space="preserve">Fundación dedicada a la promoción de la cultura y el arte en la ciudad.</t>
+  </si>
+  <si>
     <t xml:space="preserve">La Fuga es la plataforma pública de la administración distrital, que articula y gestiona la revitalización y transformación participativa del centro de Bogotá a través de su potencial creativo, el arte y la cultura.</t>
   </si>
   <si>
@@ -148,6 +196,9 @@
     <t xml:space="preserve">9c4dae24-05a5-454b-bd06-b44f7b4b5aab</t>
   </si>
   <si>
+    <t xml:space="preserve">Organización que promueve y gestiona el desarrollo cultural en Bogotá.</t>
+  </si>
+  <si>
     <t xml:space="preserve">En su calidad de entidad pública del sector Cultura Recreación y Deporte de la Alcaldía Mayor de Bogotá, el Idartes garantiza el acceso al disfrute y la práctica de las artes en condiciones de igualdad y oportunidad para los habitantes de Bogotá, mediante la promoción de la investigación, formación, creación, circulación y apropiación social del arte, potenciando la construcción de ciudadanías críticas, sensibles y creativas y las identidades culturales de la ciudad.</t>
   </si>
   <si>
@@ -163,6 +214,9 @@
     <t xml:space="preserve">26cbed04-cff6-45d8-8c3b-98ac8e94a5de</t>
   </si>
   <si>
+    <t xml:space="preserve">Instituto responsable de la protección y preservación del patrimonio cultural del distrito.</t>
+  </si>
+  <si>
     <t xml:space="preserve">El Instituto Distrital de Patrimonio Cultural (IDPC) gestiona y acompaña procesos y estrategias para la protección, intervención, divulgación, activación social y salvaguardia de los patrimonios, a escala distrital, local y barrial, mediante iniciativas de participación, diálogo y articulación social e interinstitucional que posibiliten su reconocimiento y cuidado colectivo, con enfoque territorial y poblacional-diferencial.</t>
   </si>
   <si>
@@ -178,6 +232,9 @@
     <t xml:space="preserve">6c08e1b7-e43e-42ef-ad4a-9bc3c77ed37f</t>
   </si>
   <si>
+    <t xml:space="preserve">Organismo encargado del fomento del deporte y la recreación en la ciudad.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Fomentar el bienestar integral de la ciudadanía a través de estrategias de actividad física, recreación, deporte y la sostenibilidad de parques, escenarios y equipamientos deportivos, para impulsar el desarrollo territorial, la cohesión y el tejido social. </t>
   </si>
   <si>
@@ -193,6 +250,9 @@
     <t xml:space="preserve">e819483d-de24-47eb-9b19-97a2880958fe</t>
   </si>
   <si>
+    <t xml:space="preserve">Orquesta que fomenta el desarrollo musical y artístico en Bogotá.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Cultivar y enriquecer la ciudadanía, con la interpretación y enseñanza de nuestro nutrido y diverso repertorio, por medio de la música sinfónica y el canto lirico.</t>
   </si>
   <si>
@@ -208,6 +268,9 @@
     <t xml:space="preserve">df3c6d45-a610-452f-9f01-3efae7005f0f</t>
   </si>
   <si>
+    <t xml:space="preserve">Secretaría encargada del desarrollo y promoción de la cultura, el deporte y la recreación.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Liderar la formulación e implementación concertada de políticas públicas en arte, cultura, patrimonio, recreación y deporte, así como la transformación y sostenibilidad cultural y deportiva de la ciudad, garantizando los derechos culturales, reconociendo a los habitantes de Bogotá como creadores, agentes de cambio y el centro de todas nuestras acciones en la construcción de una ciudad creadora, cuidadora, consciente e incluyente.</t>
   </si>
   <si>
@@ -226,6 +289,12 @@
     <t xml:space="preserve">Desarrollo Económico Industria y Turismo</t>
   </si>
   <si>
+    <t xml:space="preserve"> Impulsa el crecimiento económico, el apoyo a empresas y el fomento del turismo en Bogotá.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Organización dedicada a fomentar el desarrollo productivo y la competitividad en la región.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Apoyar a inversionistas que están explorando oportunidades en Bogotá y Cundinamarca</t>
   </si>
   <si>
@@ -241,6 +310,9 @@
     <t xml:space="preserve">1b09ae65-d423-41ce-bb04-76539e953cd1</t>
   </si>
   <si>
+    <t xml:space="preserve">Institución que promueve el turismo y la oferta turística de Bogotá.</t>
+  </si>
+  <si>
     <t xml:space="preserve">El Instituto Distrital de Turismo promueve el desarrollo integral y fortalecimiento económico de Bogotá, a través del turismo como integrador social, económico y mitigante del impacto ambiental; mediante políticas, planes y proyectos desde las vocaciones locales, la generación de información, la promoción de ciudad a nivel nacional e internacional como destino competitivo, sostenible, seguro, accesible e incluyente, que se articula con la región para mejorar la calidad de vida de sus habitantes y los actores de la cadena de valor del sector.</t>
   </si>
   <si>
@@ -256,6 +328,9 @@
     <t xml:space="preserve">e32446a6-18d0-481c-b2b4-3e32a9356113</t>
   </si>
   <si>
+    <t xml:space="preserve">Instituto que impulsa la economía social y el emprendimiento en la ciudad.</t>
+  </si>
+  <si>
     <t xml:space="preserve">El Instituto para la Economía Social tiene como propósito ofertar alternativas de generación de ingresos a la población de la economía informal que ejerce sus actividades en el espacio público; así como administrar y desarrollar acciones de fortalecimiento del Sistema Distrital de Plazas de Mercado, para aportar al desarrollo económico de la ciudad.</t>
   </si>
   <si>
@@ -271,6 +346,9 @@
     <t xml:space="preserve">6da76978-4091-4857-991a-24dbc6ac5894</t>
   </si>
   <si>
+    <t xml:space="preserve">Organismo responsable de la promoción del desarrollo económico y empresarial en Bogotá.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Somos la entidad Distrital que lidera la formulación, gestión y ejecución de políticas de desarrollo económico, competitividad y economía rural, orientadas a promover y fortalecer las empresas y emprendedores, el abastecimiento alimentario y la promoción de empleo y de nuevos ingresos para los ciudadanos y ciudadanas en la Bogotá -Región.</t>
   </si>
   <si>
@@ -289,6 +367,12 @@
     <t xml:space="preserve">Educación</t>
   </si>
   <si>
+    <t xml:space="preserve"> Garantiza el acceso a educación de calidad, fomenta la innovación en el aprendizaje y el desarrollo académico.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Organismo encargado de promover la educación superior, la ciencia y la tecnología en Bogotá.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Consolidar el sistema de educación y formación posmedia distrital, generando oportunidades para el acceso y permanencia a una oferta pertinente con calidad y potenciar las capacidades del ecosistema de Ciencia, Tecnología e Innovación para hacer de Bogotá una ciudad productiva, innovadora y sostenible.</t>
   </si>
   <si>
@@ -304,6 +388,9 @@
     <t xml:space="preserve">e6e31363-d0e1-4ece-bc04-b52a0896a5c3</t>
   </si>
   <si>
+    <t xml:space="preserve">Instituto enfocado en la investigación y el desarrollo pedagógico en el sector educativo.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Fortalecer y gestionar la investigación y la innovación, así como el desarrollo pedagógico y profesional docente, con miras a producir conocimiento que aporte al cierre de las brechas socioeducativas, a la garantía del derecho a la educación, a la transformación pedagógica y al reconocimiento del saber docente, para aportar en la construcción de un nuevo contrato social y ambiental.</t>
   </si>
   <si>
@@ -319,6 +406,9 @@
     <t xml:space="preserve">1da7de14-57d3-4f35-8b1e-f66c3d95aeeb</t>
   </si>
   <si>
+    <t xml:space="preserve">Secretaría responsable de la formulación y ejecución de políticas educativas en Bogotá.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Promover la oferta educativa en la ciudad para garantizar el acceso y la permanencia de los niños, niñas y jóvenes en el sistema educativo, en sus distintas formas, niveles y modalidades; la calidad y pertinencia de la educación, con el propósito de formar individuos capaces de vivir productiva, creativa y responsablemente en comunidad.</t>
   </si>
   <si>
@@ -334,6 +424,9 @@
     <t xml:space="preserve">d267f1c6-2620-4a80-815a-557a23492ba4</t>
   </si>
   <si>
+    <t xml:space="preserve">Universidad pública distrital que ofrece programas de educación superior en Bogotá.</t>
+  </si>
+  <si>
     <t xml:space="preserve">La Universidad Distrital Francisco José de Caldas es un espacio social y una organización institucional, ente autónomo del orden distrital, que tiene entre sus finalidades la formación de profesionales especializados y de ciudadanos activos; la producción y reproducción del conocimiento científico, además de la innovación tecnológica y la creación artística. Impulsa el diálogo de saberes y promueve una pedagogía, capaz de animar la reflexión y la curiosidad de los estudiantes; además, fomenta un espíritu crítico en la búsqueda de verdades abiertas; en la promoción de la ciencia y la creación; asimismo, de la ciudadanía y la democracia; y alienta la deliberación, fundada en la argumentación y en el diálogo razonado.</t>
   </si>
   <si>
@@ -352,6 +445,12 @@
     <t xml:space="preserve">Gestión Jurídica</t>
   </si>
   <si>
+    <t xml:space="preserve"> Brinda asesoría legal, garantiza el cumplimiento normativo y la defensa jurídica de entidades públicas.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entidad que asesora y representa legalmente al distrito en asuntos jurídicos.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Liderar la gestión jurídica del Distrito Capital mediante la defensa efectiva e integra de sus intereses. Promover el uso eficiente y transparente de los recursos públicos, la prevención del daño antijurídico, la promoción de la seguridad jurídica y la articulación interinstitucional, fomentando la innovación, la gestión del conocimiento y el control social para el desarrollo sostenible y la confianza ciudadana, a través de la ejecución de políticas en contratación estatal, racionalización normativa, participación ciudadana incidente, gestión judicial y disciplinaria y la representación estratégica de la ciudad en ámbitos jurídicos.</t>
   </si>
   <si>
@@ -370,6 +469,12 @@
     <t xml:space="preserve">Gestión Publica</t>
   </si>
   <si>
+    <t xml:space="preserve"> Enfocado en mejorar la administración pública, la eficiencia institucional y la transparencia gubernamental.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entidad especializada en el análisis de datos para la toma de decisiones estratégicas en el distrito.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Impulsar la toma de decisiones basadas en datos mediante la generación de soluciones analíticas para transformar la ciudad y mejorar la calidad de vida de las personas</t>
   </si>
   <si>
@@ -385,6 +490,9 @@
     <t xml:space="preserve">7e1205f0-4cd8-4e39-80fd-7651266ddc5f</t>
   </si>
   <si>
+    <t xml:space="preserve">Institución encargada de la administración del servicio civil y la gestión del talento humano.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Entidad rectora y articuladora del servicio civil en Bogotá, responsable de promover y orientar técnicamente el fortalecimiento de la Gestión Integral del Talento Humano para que responda a las necesidades de la ciudadanía.</t>
   </si>
   <si>
@@ -400,6 +508,9 @@
     <t xml:space="preserve">55d0f698-9b69-4a7f-8a64-33a3e2236f56</t>
   </si>
   <si>
+    <t xml:space="preserve">Secretaría encargada de la gestión administrativa del despacho del alcalde mayor.</t>
+  </si>
+  <si>
     <t xml:space="preserve">La Secretaría General de la Alcaldía Mayor de Bogotá, D.C., es la entidad líder del sector Gestión Pública que desarrolla condiciones para generar valor público, con el fin de lograr una ciudad moderna con un modelo de gobierno abierto, contribuir a la construcción de la paz y la reconciliación, y mejorar la calidad de vida de la ciudadanía.</t>
   </si>
   <si>
@@ -418,6 +529,12 @@
     <t xml:space="preserve">Gobierno</t>
   </si>
   <si>
+    <t xml:space="preserve"> Encargado de la gobernanza, la participación ciudadana y la administración de los asuntos públicos.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entidad responsable de la gestión y defensa del espacio público en la ciudad.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Contribuir al mejoramiento de la calidad de vida en Bogotá, por medio de una eficaz defensa del espacio público, de una óptima administración del patrimonio inmobiliario de la ciudad y de la construcción de una nueva cultura del espacio público, que garantice su uso y disfrute colectivo y estimule la participación comunitaria.</t>
   </si>
   <si>
@@ -433,6 +550,9 @@
     <t xml:space="preserve">8f2013cb-a19d-4b94-82e1-dde826049c56</t>
   </si>
   <si>
+    <t xml:space="preserve">Entidad encargada de fomentar la participación ciudadana y la acción comunal.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Somos una entidad pública, del orden distrital, que genera condiciones innovadoras, institucionales, organizativas y culturales en Bogotá y la región, que incentivan, facilitan y fortalecen la participación y el empoderamiento como forma de mejorar el bienestar de la ciudadanía y sus comunidades.</t>
   </si>
   <si>
@@ -448,6 +568,9 @@
     <t xml:space="preserve">2a1228b4-8ee2-424d-ac64-2c28d249f7f7</t>
   </si>
   <si>
+    <t xml:space="preserve">Secretaría encargada de la administración política y la gobernabilidad en la ciudad.</t>
+  </si>
+  <si>
     <t xml:space="preserve">La _Secretaría Distrital de Gobierno lidera la convivencia pacífica, el ejercicio de la ciudadanía, la promoción de la organización y de la participación ciudadana, y la coordinación de las relaciones políticas de la Administración Distrital en sus distintos niveles, para fortalecer la gobernabilidad democrática en el ámbito distrital y local, y garantizar el goce efectivo de los derechos humanos y constitucionales.</t>
   </si>
   <si>
@@ -466,6 +589,12 @@
     <t xml:space="preserve">Hábitat</t>
   </si>
   <si>
+    <t xml:space="preserve"> Responsable de la vivienda, el ordenamiento territorial y el desarrollo urbano sostenible.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Empresa prestadora de servicios de aseo y gestión de residuos en la ciudad.</t>
+  </si>
+  <si>
     <t xml:space="preserve">En Aguas de Bogotá S.A. E.S.P. prestamos servicios de gestión integral del agua, de residuos y gestión ambiental, cumpliendo con los requerimientos de nuestros clientes, a nivel nacional, contribuyendo al mejoramiento de la calidad de vida de nuestros usuarios de manera innovadora, con enfoque pedagógico, circular y sostenible.</t>
   </si>
   <si>
@@ -481,6 +610,9 @@
     <t xml:space="preserve">dae08630-74c8-44c3-906c-d4b7fdbd4bfa</t>
   </si>
   <si>
+    <t xml:space="preserve">Organismo distrital que promueve el acceso a la vivienda y el desarrollo urbano.</t>
+  </si>
+  <si>
     <t xml:space="preserve">La Caja de la Vivienda Popular tiene como misión transformar y mejorar la vivienda, el hábitat y las condiciones de vida la población de estratos 1 y 2 de Bogotá Región, a través de la implementación de los programas de Reasentamientos, Titulación de Predios y Mejoramiento de Vivienda y de Barrios, en cuyo marco desarrolla intervenciones integrales y sostenibles que reconocen las particularidades del hábitat popular. La CVP promueve el ejercicio de los derechos ciudadanos, la participación activa de la ciudadanía y el goce efectivo de la ciudad, contribuyendo a la disminución de la segregación socio espacial de la ciudad y a la mitigación de los impactos ambientales que genera la ocupación del territorio de la ciudad y su región.</t>
   </si>
   <si>
@@ -496,6 +628,9 @@
     <t xml:space="preserve">8e512352-7788-420d-9f94-e0ba1018820f</t>
   </si>
   <si>
+    <t xml:space="preserve">Empresa encargada de la prestación del servicio de acueducto y alcantarillado en Bogotá.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Agua para la vida, generando bienestar para la gente.</t>
   </si>
   <si>
@@ -511,6 +646,9 @@
     <t xml:space="preserve">622af4a0-42c7-4311-90d4-9be74fd8f599</t>
   </si>
   <si>
+    <t xml:space="preserve">Compañía que lidera la generación, distribución y comercialización de energía en la ciudad.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Gestionar sistemas de transmisión, transporte y distribución, así como inversiones en el sector energético</t>
   </si>
   <si>
@@ -526,6 +664,9 @@
     <t xml:space="preserve">1d8d452b-c609-4ae7-9b8c-567a1f28032f</t>
   </si>
   <si>
+    <t xml:space="preserve">Entidad responsable de la renovación y el desarrollo urbano en Bogotá.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Somos el operador de proyectos de revitalización urbana de Bogotá. Identificamos, promovemos, gestionamos, gerenciamos y ejecutamos proyectos integrales para el desarrollo de las ciudades.</t>
   </si>
   <si>
@@ -541,6 +682,9 @@
     <t xml:space="preserve">5ae28390-f8b2-43cd-a3ba-cf0c8303517f</t>
   </si>
   <si>
+    <t xml:space="preserve">Empresa que gestiona la infraestructura de telecomunicaciones del distrito.</t>
+  </si>
+  <si>
     <t xml:space="preserve">La misión de ETB es entregar soluciones integrales de tecnologías de información y comunicaciones que satisfacen a nuestros clientes y contribuyen al fortalecimiento de la sociedad de la información, en el marco de la Responsabilidad Social Empresarial</t>
   </si>
   <si>
@@ -556,6 +700,9 @@
     <t xml:space="preserve">6b9496af-f22b-4ffa-8fd0-3715b7a4c44f</t>
   </si>
   <si>
+    <t xml:space="preserve">Entidad responsable de la planificación y ejecución de políticas de vivienda.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Somos la entidad cabeza del Sector Hábitat encargada de liderar la formulación e implementación de políticas de gestión del territorio urbano y rural, con un enfoque de mejoramiento integral; para promover la vivienda digna, y facilitar el acceso a espacios y servicios públicos en el Distrito Capital.</t>
   </si>
   <si>
@@ -571,6 +718,9 @@
     <t xml:space="preserve">f40536a4-9859-440c-8dbe-6de07ea0c57f</t>
   </si>
   <si>
+    <t xml:space="preserve">Entidad que administra los servicios públicos y la gestión de residuos sólidos.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Garantizar en el Distrito Capital la prestación, coordinación, supervisión, gestión, monitoreo y control de los servicios públicos de aseo en sus componentes (recolección, barrido y limpieza, disposición final y aprovechamiento de residuos sólidos), los residuos de construcción y demolición, los servicios funerarios y el servicio de alumbrado público; defendiendo el carácter público de la infraestructura propiedad del Distrito, promoviendo la participación ciudadana en la gestión pública, mejorando la calidad de vida de sus ciudadanos y el cuidado del medio ambiente a través de la planeación y modelación de los servicios a cargo.</t>
   </si>
   <si>
@@ -589,6 +739,12 @@
     <t xml:space="preserve">Hacienda</t>
   </si>
   <si>
+    <t xml:space="preserve"> Maneja las finanzas públicas, el presupuesto distrital, la tributación y las políticas económicas.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fondo encargado de la administración de pensiones y cesantías de los servidores públicos.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Somos el Fondo de Prestaciones Económicas, Cesantías y Pensiones de Bogotá, FONCEP, que garantiza el reconocimiento de los derechos prestacionales y el pago de las obligaciones pensionales a nuestros afiliados, con el fin de brindarles amparo en la vejez, invalidez y sobrevivencia a favor de sus beneficiarios.</t>
   </si>
   <si>
@@ -604,6 +760,9 @@
     <t xml:space="preserve">de5e850e-a009-496c-b5cf-61ecefd9daf7</t>
   </si>
   <si>
+    <t xml:space="preserve">Entidad encargada de la operación y administración de la lotería de Bogotá.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Somos diversión y cumplimos sueños, fomentando los juegos de suerte y azar responsablemente, contribuyendo a la salud de los colombianos; trabajamos de la mano de nuestros clientes, colaboradores, distribuidores, y grupos de valor..</t>
   </si>
   <si>
@@ -619,6 +778,9 @@
     <t xml:space="preserve">d8ee456f-f58d-423b-9407-1af8f7ee5faa</t>
   </si>
   <si>
+    <t xml:space="preserve">Secretaría que gestiona los recursos financieros y el presupuesto distrital.</t>
+  </si>
+  <si>
     <t xml:space="preserve">La Secretaría Distrital de Hacienda tiene la misión de contribuir al desarrollo sostenible de Bogotá y al mejoramiento de la calidad de vida de sus habitantes, mediante una recaudación eficiente y distribución efectiva de recursos, para la implementación de políticas y proyectos de alto impacto.</t>
   </si>
   <si>
@@ -634,6 +796,9 @@
     <t xml:space="preserve">5026a6c5-bc28-4abe-ba16-84848fd70f3f</t>
   </si>
   <si>
+    <t xml:space="preserve">Entidad encargada de la gestión y actualización del catastro en Bogotá.</t>
+  </si>
+  <si>
     <t xml:space="preserve">La Unidad Administrativa Especial de Catastro Distrital es la entidad encargada de recopilar, integrar y disponer la información georreferenciada de la propiedad inmueble del Distrito Capital en sus aspectos físico, jurídico y económico, que contribuya a la planeación económica, social y territorial del Distrito Capital permitiendo la satisfacción de los grupos de valor.</t>
   </si>
   <si>
@@ -652,6 +817,12 @@
     <t xml:space="preserve">Integración Social</t>
   </si>
   <si>
+    <t xml:space="preserve"> Diseña políticas y programas para la inclusión social y el apoyo a poblaciones vulnerables.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entidad encargada de la protección y atención integral de la niñez y juventud.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Formar ciudadanos creativos e innovadores con oportunidades, desde un modelo pedagógico basado en los principios de afecto, alegría y libertad y un talento institucional que apropia la vocación de servicio y liderazgo para construir proyecto y sentido de vida en los niños, niñas, adolescentes y jóvenes en habitabilidad en calle, en riesgo de habitarla o en condiciones de fragilidad social de la Ciudad.</t>
   </si>
   <si>
@@ -667,6 +838,9 @@
     <t xml:space="preserve">deca3f0e-aeac-4446-8e7c-793ba8cb2bb2</t>
   </si>
   <si>
+    <t xml:space="preserve">Entidad encargada de la integración y protección social de poblaciones vulnerables.</t>
+  </si>
+  <si>
     <t xml:space="preserve">La Secretaría Distrital de Integración Social, es una entidad pública de nivel central de la ciudad de Bogotá, líder del sector social, responsable de la formulación e implementación de políticas públicas poblacionales orientadas al ejercicio de derechos, ofrece servicios sociales y promueve de forma articulada, la inclusión social, el desarrollo de capacidades y la mejora en la calidad de vida de la población en mayor condición de vulnerabilidad, con un enfoque territorial.</t>
   </si>
   <si>
@@ -685,6 +859,12 @@
     <t xml:space="preserve">Movilidad</t>
   </si>
   <si>
+    <t xml:space="preserve"> Planifica y administra la infraestructura de transporte, el sistema de movilidad y el tránsito en Bogotá.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entidad a cargo de la operación del sistema de transporte público masivo TransMilenio.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Somos los responsables de gestionar el Sistema Integrado de Transporte Público de Bogotá D.C., en sus componentes troncal, zonal, alimentación y cable, que conecta a las personas con las oportunidades que brinda la ciudad, en condiciones de calidad, seguridad y eficiencia.</t>
   </si>
   <si>
@@ -700,6 +880,9 @@
     <t xml:space="preserve">a835f2e5-8516-4942-8526-44d7338480bc</t>
   </si>
   <si>
+    <t xml:space="preserve">Empresa encargada del desarrollo, operación y gestión del metro de Bogotá.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Nuestro propósito como Empresa Metro de Bogotá es transformar positivamente la movilidad del Distrito Capital mediante la implementación y operación del modo ferroviario del SITP; con conexión a las redes de integración regional, aportando al desarrollo y renovación urbana de la ciudad, con el fin de generar acceso a oportunidades urbanas y mejorar la calidad de vida de los ciudadanos.</t>
   </si>
   <si>
@@ -715,6 +898,9 @@
     <t xml:space="preserve">93c5d9a1-9971-4450-ab5a-66a350eb158a</t>
   </si>
   <si>
+    <t xml:space="preserve">Instituto encargado de la planificación y ejecución de proyectos de infraestructura vial.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Estructuramos y desarrollamos proyectos de infraestructura vial y movilidad multimodal, de forma sostenible, incluyente, innovadora y eficiente, para contribuir al desarrollo urbano de Bogotá Región y mejorar la calidad de vida de su gente.</t>
   </si>
   <si>
@@ -730,6 +916,9 @@
     <t xml:space="preserve">05c61cf4-3560-4f3c-99db-9c3f9787a2f7</t>
   </si>
   <si>
+    <t xml:space="preserve">Operadora responsable del sistema de transporte público en la ciudad.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Prestar un servicio de transporte multimodal de alta calidad, innovador, eficiente y sostenible, que contribuya a la mejora de la calidad de vida de nuestras usuarias, usuarios y colaboradores aportando al cuidado del medio ambiente, el desarrollo social y económico de Bogotá y su área de influencia.</t>
   </si>
   <si>
@@ -745,6 +934,9 @@
     <t xml:space="preserve">c4f36231-7247-483a-b21e-44e5d118db29</t>
   </si>
   <si>
+    <t xml:space="preserve">Entidad encargada de la planificación y regulación de la movilidad en Bogotá.</t>
+  </si>
+  <si>
     <t xml:space="preserve">La Secretaría Distrital de Movilidad como líder del sector, formula políticas e implementa estrategias de movilidad multimodal, incluyente y sostenible que contribuyen a la equidad y mejoran la calidad de vida de la ciudadanía y la seguridad de los actores viales, potenciando la productividad, la competitividad y la integración de Bogotá y la región, con una gestión íntegra y transparente.</t>
   </si>
   <si>
@@ -760,6 +952,9 @@
     <t xml:space="preserve">c2100c35-c6cf-405e-9861-cf159c5697c5</t>
   </si>
   <si>
+    <t xml:space="preserve">Entidad responsable de la operación y administración de la terminal de transportes.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Promover, desarrollar y explotar soluciones de movilidad, mediante la gestión y operación innovadora, eficiente y sostenible de servicios a la ciudadanía, al sector transportador, regional y privado, que impacten positivamente en la movilidad distrital y/o nacional.</t>
   </si>
   <si>
@@ -775,6 +970,9 @@
     <t xml:space="preserve">ce0f66f7-a7ad-4e4f-a631-f083237dcc0a</t>
   </si>
   <si>
+    <t xml:space="preserve">Institución responsable del mantenimiento y rehabilitación de la infraestructura vial.</t>
+  </si>
+  <si>
     <t xml:space="preserve">La misión de la Unidad Administrativa Especial de Rehabilitación y Mantenimiento Vial (UAERMV) de Bogotá es mejorar la movilidad y disminuir la accidentalidad en la ciudad: Conservar la malla vial local, Atender situaciones imprevistas que dificultan la movilidad, Brindar apoyo interinstitucional.  </t>
   </si>
   <si>
@@ -793,6 +991,12 @@
     <t xml:space="preserve">Mujeres</t>
   </si>
   <si>
+    <t xml:space="preserve"> Formula e implementa políticas de equidad de género, derechos de las mujeres y empoderamiento femenino.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Secretaría que fomenta la equidad de género y los derechos de las mujeres.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Liderar, orientar y coordinar la formulación, implementación, seguimiento y evaluación de la Política Pública de Mujeres y Equidad de Género, así como la transversalización de los enfoques de derechos de las mujeres, de género y diferencial, en los planes, programas, proyectos y políticas públicas distritales, para la protección, garantía y materialización de los derechos humanos de las mujeres en las diferencias y diversidades que las constituyen, promoviendo su autonomía y el ejercicio pleno de su ciudadanía en el Distrito Capital</t>
   </si>
   <si>
@@ -811,6 +1015,12 @@
     <t xml:space="preserve">Órganos de Control</t>
   </si>
   <si>
+    <t xml:space="preserve"> Entidades encargadas de la vigilancia, control y auditoría de la gestión pública.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Órgano de representación y deliberación que formula normas y políticas distritales.</t>
+  </si>
+  <si>
     <t xml:space="preserve">El Concejo de Bogotá D.C. como Suprema Autoridad Política Administrativa del Distrito Capital, expide normas que promueven el desarrollo integral de sus habitantes y de la ciudad, así mismo, vigila la gestión de la Administración Distrital, como así mismo elige a los servidores públicos distritales conforme a lo establecido en el Reglamento Interno del Concejo y la normatividad vigente.</t>
   </si>
   <si>
@@ -826,6 +1036,9 @@
     <t xml:space="preserve">44d84dd4-805e-4a0a-955b-8587e5c661fc</t>
   </si>
   <si>
+    <t xml:space="preserve">Entidad encargada de la fiscalización y control del uso de los recursos públicos en Bogotá.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Vigilamos la gestión de los recursos del Distrito Capital con oportunidad y efectividad, apoyados en el control social participativo, alianzas estratégicas e innovación tecnológica, para contribuir al mejoramiento de la calidad de vida de los ciudadanos. </t>
   </si>
   <si>
@@ -841,6 +1054,9 @@
     <t xml:space="preserve">ccb07bc2-67b9-4c6b-9d1e-8d84493cde19</t>
   </si>
   <si>
+    <t xml:space="preserve">Organismo encargado de la vigilancia y control de la administración distrital.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Como órgano de control, la Personería de Bogotá, D. C., ejerce funciones de Ministerio Público, defensor de los derechos humanos que vigila la conducta de los servidores públicos, actuando de manera oportuna y resolutiva para garantizar el respeto de los derechos fundamentales, el cumplimiento de las funciones misionales y la normatividad vigente y el buen funcionamiento de las instituciones públicas en beneficio de las partes interesadas.</t>
   </si>
   <si>
@@ -856,6 +1072,9 @@
     <t xml:space="preserve">1b01632f-f169-46c5-be3a-d1c1eee6f58c</t>
   </si>
   <si>
+    <t xml:space="preserve">Organismo encargado del control ciudadano y la vigilancia de la gestión pública.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Somos un organismo autónomo de control y vigilancia, de carácter asesor y preventivo, encargado de contribuir con sus acciones a la eficiencia y transparencia de las entidades distritales, la participación ciudadana y el control social para incentivar la confianza en la gestión pública.</t>
   </si>
   <si>
@@ -874,6 +1093,12 @@
     <t xml:space="preserve">Planeación</t>
   </si>
   <si>
+    <t xml:space="preserve"> Responsable del diseño y ejecución de planes estratégicos y de desarrollo en la ciudad.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Secretaría que dirige la planificación territorial y el desarrollo urbano de la ciudad.</t>
+  </si>
+  <si>
     <t xml:space="preserve">En la SDP planeamos y orientamos la transformación - territorial, económica, social y ambiental – del distrito capital para mejorar el bienestar colectivo y la competitividad de nuestra ciudad región - incluyente, cuidadora, equitativa y solidaria -, a través de las políticas públicas, la participación ciudadana y una gestión pública efectiva, digital e innovadora.</t>
   </si>
   <si>
@@ -892,6 +1117,12 @@
     <t xml:space="preserve">Salud</t>
   </si>
   <si>
+    <t xml:space="preserve"> Administra los servicios de salud pública, la prevención de enfermedades y la atención médica.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entidad de salud enfocada en la prestación de servicios médicos a los ciudadanos.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Somos la EPS que garantiza el aseguramiento, el bienestar y la salud de sus afiliados; basada en un modelo de atención integral en salud, con altos estándares de calidad, trato humanizado, renovación tecnológica, con un equipo de trabajo competente enfocada en la satisfacción de nuestros afiliados y sus familias.</t>
   </si>
   <si>
@@ -907,6 +1138,9 @@
     <t xml:space="preserve">b1b5b22b-fd6e-4bfe-8c94-aee4718f7749</t>
   </si>
   <si>
+    <t xml:space="preserve">Centro especializado en el desarrollo y producción de vacunas en el distrito.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Celebrar y ejecutar contratos para la investigación y desarrollo de biológicos. Construir, instalar, administrar, modificar y operar plantas, laboratorios, fábricas o centros para el desarrollo y producción de biológicos.</t>
   </si>
   <si>
@@ -922,6 +1156,9 @@
     <t xml:space="preserve">a735fee7-3139-4cbf-9eb4-88a51e2d69f9</t>
   </si>
   <si>
+    <t xml:space="preserve">Institución que apoya la gestión administrativa y técnica del distrito.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Somos una entidad que gestiona procesos de contratación de bienes y servicios para entidades públicas y privadas del sector salud de orden Distrital y Nacional, de manera transparente, objetiva, eficiente y responsable.</t>
   </si>
   <si>
@@ -937,6 +1174,9 @@
     <t xml:space="preserve">79b706db-7008-402f-a268-2e796aee894c</t>
   </si>
   <si>
+    <t xml:space="preserve">Entidad que administra los recursos financieros del sector salud en Bogotá.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Recaudar y administrar los recursos que son captados por Bogotá y que provienen de diferentes fuentes públicas y privadas, destinadas al sector salud.</t>
   </si>
   <si>
@@ -952,6 +1192,9 @@
     <t xml:space="preserve">b9aed058-7ae7-47b1-aa6d-57382a7df8af</t>
   </si>
   <si>
+    <t xml:space="preserve">Instituto especializado en la investigación y desarrollo en biotecnología y salud.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Somos un instituto de ciencia, tecnología e innovación en salud, con énfasis en investigación médica y biotecnológica, que genera conocimiento y desarrollo científico, sobre la base del fortalecimiento de las capacidades del talento humano, infraestructura, cultura de la calidad y compromiso social, para la gestión de conocimiento y la provisión de productos e insumos biológicos humanos al servicio de la población.</t>
   </si>
   <si>
@@ -967,6 +1210,9 @@
     <t xml:space="preserve">289452a5-d96a-41a2-89f0-a16058a70511</t>
   </si>
   <si>
+    <t xml:space="preserve">Organismo responsable de la formulación y ejecución de políticas de salud pública.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Somos la entidad rectora de salud en Bogotá, constituida por un equipo humano comprometido con la excelencia, responsable de garantizar el ejercicio efectivo del derecho a la salud de toda la población, a través de la implementación de un modelo de atención integral, equitativa, universal, participativa, centrada en el ser humano, la responsabilidad social y la sostenibilidad ambiental.</t>
   </si>
   <si>
@@ -982,6 +1228,9 @@
     <t xml:space="preserve">924f505e-b985-4139-a03f-2075e23075d0</t>
   </si>
   <si>
+    <t xml:space="preserve">Red hospitalaria que presta servicios de salud en la zona centro-oriente de Bogotá.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Somos la Subred Integrada de Servicios de Salud Centro Oriente del Distrito Capital, prestamos servicios de salud en el marco de una gestión clínica segura con estándares superiores de calidad, trato humanizado, mejoramiento continuo, gestión interinstitucional e intersectorial, participación comunitaria y generación del conocimiento por medio de la investigación y la docencia para impactar las condiciones de salud de usuarios, familias y comunidades, con talento humano íntegro y calificado.</t>
   </si>
   <si>
@@ -997,6 +1246,9 @@
     <t xml:space="preserve">da3ccecf-b7ad-46f2-a759-edd4533cd47c</t>
   </si>
   <si>
+    <t xml:space="preserve">Red de hospitales que ofrece atención médica en la zona norte de la ciudad.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Somos una Empresa Social del Estado innovadora y socialmente responsable, que presta servicios de salud integrales y de calidad, con participación activa en la formación de talento humano y desarrollo de la docencia y la investigación, contribuyendo al mejoramiento de la calidad de vida de la población.</t>
   </si>
   <si>
@@ -1012,6 +1264,9 @@
     <t xml:space="preserve">69a66e34-418d-4f80-85cd-f9510d2d524e</t>
   </si>
   <si>
+    <t xml:space="preserve">Red hospitalaria enfocada en la prestación de servicios de salud en la zona sur.</t>
+  </si>
+  <si>
     <t xml:space="preserve">La Subred Integrada de Servicios de Salud Sur E.S.E., presta Servicios de Salud a través de un Modelo de Atención Integral en Red, bajo los enfoques de gestión integral del riesgo y seguridad, fortaleciendo la formación académica orientada a la investigación científica e innovación, con un talento humano comprometido, humanizado y competente que contribuye al mejoramiento de las condiciones de salud de nuestros usuarios urbanos y rurales de las localidades de Usme, Ciudad Bolívar, Tunjuelito y Sumapaz.</t>
   </si>
   <si>
@@ -1027,6 +1282,9 @@
     <t xml:space="preserve">a6fa44d1-a682-4599-8e12-a0f1a12b6b69</t>
   </si>
   <si>
+    <t xml:space="preserve">Red integrada de salud que atiende a la población en el suroccidente de Bogotá.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Brindar servicios de salud con altos estándares de calidad, a través del Modelo de Atención Integral basado en Atención Primaria en Salud, gestión asistencial excelente, segura, humanizada, eficiente, promoción de la docencia, investigación e innovación con talento humano íntegro para contribuir al bienestar y calidad de vida de la población.</t>
   </si>
   <si>
@@ -1045,6 +1303,12 @@
     <t xml:space="preserve">Sector descentralizado territorialmente</t>
   </si>
   <si>
+    <t xml:space="preserve"> Conformado por las 20 alcaldías locales de Bogotá, encargadas de la gestión territorial en sus respectivas localidades.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Administración local encargada de la gestión y desarrollo del territorio de Antonio Nariño.</t>
+  </si>
+  <si>
     <t xml:space="preserve">La Secretaría Distrital de Gobierno lidera la convivencia pacífica, el ejercicio de la ciudadanía, la promoción de la organización y de la participación ciudadana, y la coordinación de las relaciones políticas de la Administración Distrital en sus distintos niveles, para fortalecer la gobernabilidad democrática en el ámbito distrital y local, y garantizar el goce efectivo de los derechos humanos y constitucionales.</t>
   </si>
   <si>
@@ -1057,6 +1321,9 @@
     <t xml:space="preserve">6e2f4e1e-b26e-497d-b6f0-bf30f162c1dc</t>
   </si>
   <si>
+    <t xml:space="preserve">Entidad gubernamental responsable de la administración de la localidad de Barrios Unidos.</t>
+  </si>
+  <si>
     <t xml:space="preserve">http://www.barriosunidos.gov.co/transparencia/organizacion/quienes-somos</t>
   </si>
   <si>
@@ -1066,6 +1333,9 @@
     <t xml:space="preserve">b00a799a-4c7e-449c-9eb8-8f3d4123e788</t>
   </si>
   <si>
+    <t xml:space="preserve">Alcaldía local encargada de la planificación y gestión de la localidad de Bosa.</t>
+  </si>
+  <si>
     <t xml:space="preserve">http://bosa.gov.co/transparencia/organizacion/quienes-somos</t>
   </si>
   <si>
@@ -1075,6 +1345,9 @@
     <t xml:space="preserve">637445a7-7ee6-44a7-b053-a613f873248f</t>
   </si>
   <si>
+    <t xml:space="preserve">Administración local que gestiona el desarrollo urbano y social de Chapinero.</t>
+  </si>
+  <si>
     <t xml:space="preserve">http://www.chapinero.gov.co/transparencia/organizacion/quienes-somos</t>
   </si>
   <si>
@@ -1084,6 +1357,9 @@
     <t xml:space="preserve">82e05c17-326b-46a1-a875-62fb9db97e0b</t>
   </si>
   <si>
+    <t xml:space="preserve">Entidad que dirige y administra los servicios y proyectos en Ciudad Bolívar.</t>
+  </si>
+  <si>
     <t xml:space="preserve">http://www.ciudadbolivar.gov.co/transparencia/organizacion/quienes-somos</t>
   </si>
   <si>
@@ -1093,6 +1369,9 @@
     <t xml:space="preserve">f4f22688-fb8a-40ba-b58b-13d334dbf897</t>
   </si>
   <si>
+    <t xml:space="preserve">Alcaldía que supervisa y gestiona el desarrollo de la localidad de Engativá.</t>
+  </si>
+  <si>
     <t xml:space="preserve">http://www.engativa.gov.co/transparencia/organizacion/quienes-somos</t>
   </si>
   <si>
@@ -1102,6 +1381,9 @@
     <t xml:space="preserve">1b8fefa0-afe4-4c6e-9a13-e15c39b76a4e</t>
   </si>
   <si>
+    <t xml:space="preserve">Entidad responsable de la planificación y administración de la localidad de Fontibón.</t>
+  </si>
+  <si>
     <t xml:space="preserve">http://www.fontibon.gov.co/transparencia/organizacion/quienes-somos</t>
   </si>
   <si>
@@ -1111,6 +1393,9 @@
     <t xml:space="preserve">d65b7bcc-d53a-4543-a294-6f52e146281d</t>
   </si>
   <si>
+    <t xml:space="preserve">Alcaldía encargada de la gestión territorial y el desarrollo comunitario en Kennedy.</t>
+  </si>
+  <si>
     <t xml:space="preserve">http://kennedy.gov.co/transparencia/organizacion/quienes-somos</t>
   </si>
   <si>
@@ -1120,6 +1405,9 @@
     <t xml:space="preserve">3563fdd5-9aeb-4b80-804f-ab21beaf454f</t>
   </si>
   <si>
+    <t xml:space="preserve">Entidad que vela por el desarrollo urbano y social de La Candelaria.</t>
+  </si>
+  <si>
     <t xml:space="preserve">http://www.lacandelaria.gov.co/transparencia/organizacion/quienes-somos</t>
   </si>
   <si>
@@ -1129,6 +1417,9 @@
     <t xml:space="preserve">35492fe1-7cc7-4e86-a18c-aa42d2e6469c</t>
   </si>
   <si>
+    <t xml:space="preserve">Administración local responsable de la planificación y ejecución de proyectos en Los Mártires.</t>
+  </si>
+  <si>
     <t xml:space="preserve">http://martires.gov.co/transparencia/organizacion/quienes-somos</t>
   </si>
   <si>
@@ -1138,6 +1429,9 @@
     <t xml:space="preserve">0ac22659-e454-444e-9333-9e0b6b1731c6</t>
   </si>
   <si>
+    <t xml:space="preserve">Alcaldía local que gestiona el desarrollo de Puente Aranda y sus comunidades.</t>
+  </si>
+  <si>
     <t xml:space="preserve">http://puentearanda.gov.co/transparencia/organizacion/quienes-somos</t>
   </si>
   <si>
@@ -1147,6 +1441,9 @@
     <t xml:space="preserve">16790b2a-7734-4ee5-8914-a100e6c136cb</t>
   </si>
   <si>
+    <t xml:space="preserve">Entidad encargada del bienestar y la infraestructura de Rafael Uribe Uribe.</t>
+  </si>
+  <si>
     <t xml:space="preserve">http://www.rafaeluribe.gov.co/transparencia/organizacion/quienes-somos</t>
   </si>
   <si>
@@ -1156,6 +1453,9 @@
     <t xml:space="preserve">0567f60c-47f5-43ce-a028-b80eaf88d37a</t>
   </si>
   <si>
+    <t xml:space="preserve">Administración que supervisa el desarrollo de la localidad de San Cristóbal.</t>
+  </si>
+  <si>
     <t xml:space="preserve">http://sancristobal.gov.co/transparencia/organizacion/quienes-somos</t>
   </si>
   <si>
@@ -1165,6 +1465,9 @@
     <t xml:space="preserve">6d0b0be5-3af2-488e-9584-bdd829b27c40</t>
   </si>
   <si>
+    <t xml:space="preserve">Alcaldía responsable de la gestión territorial y social en Santa Fe.</t>
+  </si>
+  <si>
     <t xml:space="preserve">http://santafe.gov.co/transparencia/organizacion/quienes-somos</t>
   </si>
   <si>
@@ -1174,6 +1477,9 @@
     <t xml:space="preserve">d4736ade-3144-4127-bd1f-a428c77e125e</t>
   </si>
   <si>
+    <t xml:space="preserve">Entidad encargada de la administración y desarrollo de la localidad de Suba.</t>
+  </si>
+  <si>
     <t xml:space="preserve">http://suba.gov.co/transparencia/organizacion/quienes-somos</t>
   </si>
   <si>
@@ -1183,6 +1489,9 @@
     <t xml:space="preserve">f1e3fb07-af80-40e9-b3ba-951392680ceb</t>
   </si>
   <si>
+    <t xml:space="preserve">Alcaldía que gestiona el desarrollo territorial y comunitario en Sumapaz.</t>
+  </si>
+  <si>
     <t xml:space="preserve">http://sumapaz.gov.co/transparencia/organizacion/quienes-somos</t>
   </si>
   <si>
@@ -1192,6 +1501,9 @@
     <t xml:space="preserve">29b462d1-a002-4c07-a854-1c82fc10829f</t>
   </si>
   <si>
+    <t xml:space="preserve">Administración local encargada de la planificación y ejecución de proyectos en Teusaquillo.</t>
+  </si>
+  <si>
     <t xml:space="preserve">http://teusaquillo.gov.co/transparencia/organizacion/quienes-somos</t>
   </si>
   <si>
@@ -1201,6 +1513,9 @@
     <t xml:space="preserve">1dcd0622-9833-4ca8-8b09-ea7617ead3c3</t>
   </si>
   <si>
+    <t xml:space="preserve">Entidad responsable del desarrollo urbano y social en Tunjuelito.</t>
+  </si>
+  <si>
     <t xml:space="preserve">http://www.tunjuelito.gov.co/transparencia/organizacion/quienes-somos</t>
   </si>
   <si>
@@ -1210,6 +1525,9 @@
     <t xml:space="preserve">31b7d251-5580-45d3-9e5b-e76853b78302</t>
   </si>
   <si>
+    <t xml:space="preserve">Alcaldía local encargada del desarrollo de la comunidad en Usaquén.</t>
+  </si>
+  <si>
     <t xml:space="preserve">http://www.usaquen.gov.co/transparencia/organizacion/quienes-somos</t>
   </si>
   <si>
@@ -1219,6 +1537,9 @@
     <t xml:space="preserve">aee6112d-44a4-4cca-876c-fcde6582e9f2</t>
   </si>
   <si>
+    <t xml:space="preserve">Entidad encargada de la gestión y planificación de la localidad de Usme.</t>
+  </si>
+  <si>
     <t xml:space="preserve">http://www.usme.gov.co/transparencia/organizacion/quienes-somos</t>
   </si>
   <si>
@@ -1231,6 +1552,12 @@
     <t xml:space="preserve">Seguridad Convivencia y Justicia</t>
   </si>
   <si>
+    <t xml:space="preserve"> Se ocupa de la seguridad ciudadana, la justicia, la prevención del delito y la resolución de conflictos.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entidad a cargo de la seguridad, la convivencia y la justicia en el distrito.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Liderar, planear, implementar y evaluar la política pública en materia de seguridad, convivencia y acceso a la justicia, así como gestionar los servicios de emergencias, para garantizar el ejercicio de los derechos y libertades de los ciudadanos del Distrito Capital.</t>
   </si>
   <si>
@@ -1244,6 +1571,9 @@
   </si>
   <si>
     <t xml:space="preserve">e4cd18f0-b93e-43e3-9e70-b67b5b86101d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cuerpo oficial encargado de la prevención y atención de emergencias de bomberos.</t>
   </si>
   <si>
     <t xml:space="preserve">Proteger la vida, el ambiente y el patrimonio, a través de la gestión integral de riesgos de incendios, atención de rescates en todas sus modalidades e incidentes con materiales peligrosos en Bogotá y su entorno</t>
@@ -1262,7 +1592,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1284,6 +1614,19 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
@@ -1335,11 +1678,11 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1352,7 +1695,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1635,19 +1982,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G86"/>
+  <dimension ref="A1:I86"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.71484375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.71484375" defaultRowHeight="12.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="97.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="35.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="1" width="90.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16135" style="1" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="4" style="1" width="90.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16137" style="1" width="11.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1672,1971 +2019,2487 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="1" t="n">
+        <v>2030</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="D3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="1" t="n">
-        <v>2030</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="1" t="n">
+      <c r="E3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="1" t="n">
         <v>2093</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" s="1" t="n">
         <v>2046</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G5" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I5" s="1" t="n">
         <v>2050</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="G6" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="I6" s="1" t="n">
         <v>2026</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I7" s="1" t="n">
+        <v>2049</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="D8" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G7" s="1" t="n">
-        <v>2049</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="G8" s="1" t="n">
+      <c r="E8" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="I8" s="1" t="n">
         <v>2036</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="G9" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I9" s="1" t="n">
         <v>2031</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G10" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="I10" s="1" t="n">
         <v>2040</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>57</v>
+        <v>38</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="G11" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="I11" s="1" t="n">
         <v>2107</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G12" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="I12" s="1" t="n">
         <v>2078</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>68</v>
+        <v>82</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>83</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="G13" s="1" t="n">
+        <v>84</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="I13" s="1" t="n">
         <v>2104</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>71</v>
+        <v>88</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="G14" s="1" t="n">
+        <v>82</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="I14" s="1" t="n">
         <v>2032</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>75</v>
+        <v>93</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>76</v>
+        <v>94</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="G15" s="1" t="n">
+        <v>82</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="I15" s="1" t="n">
         <v>2033</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>80</v>
+        <v>99</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="G16" s="1" t="n">
+      <c r="E16" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="I16" s="1" t="n">
         <v>2090</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>85</v>
+        <v>105</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>86</v>
+        <v>106</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>87</v>
+        <v>107</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="G17" s="1" t="n">
+        <v>108</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="I17" s="1" t="n">
         <v>2028</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>91</v>
+        <v>113</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>92</v>
+        <v>114</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>87</v>
+        <v>107</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="G18" s="1" t="n">
+        <v>108</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="I18" s="1" t="n">
         <v>2042</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>96</v>
+        <v>119</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>97</v>
+        <v>120</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>87</v>
+        <v>107</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="G19" s="1" t="n">
+        <v>108</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="I19" s="1" t="n">
         <v>2083</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>101</v>
+        <v>125</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>102</v>
+        <v>126</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>87</v>
+        <v>107</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="G20" s="1" t="n">
+        <v>108</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="I20" s="1" t="n">
         <v>2077</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>106</v>
+        <v>131</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>107</v>
+        <v>132</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>108</v>
+        <v>133</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="G21" s="1" t="n">
+        <v>134</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="I21" s="1" t="n">
         <v>2094</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>112</v>
+        <v>139</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>113</v>
+        <v>140</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>114</v>
+        <v>141</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="G22" s="1" t="n">
+        <v>142</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="I22" s="1" t="n">
         <v>2045</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>118</v>
+        <v>147</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>119</v>
+        <v>148</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>114</v>
+        <v>141</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="G23" s="1" t="n">
+        <v>142</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="I23" s="1" t="n">
         <v>2037</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>123</v>
+        <v>153</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>124</v>
+        <v>154</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>114</v>
+        <v>141</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="G24" s="1" t="n">
+        <v>142</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="I24" s="1" t="n">
         <v>2074</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>128</v>
+        <v>159</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>129</v>
+        <v>160</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>130</v>
+        <v>161</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="G25" s="1" t="n">
+        <v>162</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="I25" s="1" t="n">
         <v>2029</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>134</v>
+        <v>167</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>135</v>
+        <v>168</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>130</v>
+        <v>161</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="G26" s="1" t="n">
+        <v>162</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="I26" s="1" t="n">
         <v>2100</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>139</v>
+        <v>173</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>140</v>
+        <v>174</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>130</v>
+        <v>161</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="G27" s="1" t="n">
+        <v>162</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="I27" s="1" t="n">
         <v>2047</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>144</v>
+        <v>179</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>145</v>
+        <v>180</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>146</v>
+        <v>181</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="G28" s="1" t="n">
+        <v>182</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="I28" s="1" t="n">
         <v>2034</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>150</v>
+        <v>187</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>151</v>
+        <v>188</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>146</v>
+        <v>181</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="G29" s="1" t="n">
+        <v>182</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="I29" s="1" t="n">
         <v>2048</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>155</v>
+        <v>193</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>156</v>
+        <v>194</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>146</v>
+        <v>181</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="G30" s="1" t="n">
+        <v>182</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="I30" s="1" t="n">
         <v>2024</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>160</v>
+        <v>199</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>161</v>
+        <v>200</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>146</v>
+        <v>181</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="G31" s="1" t="n">
+        <v>182</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="I31" s="1" t="n">
         <v>2044</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>165</v>
+        <v>205</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>166</v>
+        <v>206</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>146</v>
+        <v>181</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="G32" s="1" t="n">
+        <v>182</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="H32" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="I32" s="1" t="n">
         <v>2088</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>170</v>
+        <v>211</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>171</v>
+        <v>212</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>146</v>
+        <v>181</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>173</v>
+        <v>182</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>213</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="G33" s="1" t="n">
+        <v>214</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="I33" s="1" t="n">
         <v>2105</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>175</v>
+        <v>217</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>176</v>
+        <v>218</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>146</v>
+        <v>181</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="G34" s="1" t="n">
+        <v>182</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="I34" s="1" t="n">
         <v>2089</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>180</v>
+        <v>223</v>
       </c>
       <c r="B35" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>181</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>146</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="E35" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="G35" s="1" t="n">
+      <c r="E35" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="H35" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="I35" s="1" t="n">
         <v>2043</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>185</v>
+        <v>229</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>186</v>
+        <v>230</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>187</v>
+        <v>231</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="G36" s="1" t="n">
+        <v>232</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="H36" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="I36" s="1" t="n">
         <v>2087</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>191</v>
+        <v>237</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>192</v>
+        <v>238</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>187</v>
+        <v>231</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="F37" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="G37" s="1" t="n">
+        <v>232</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="H37" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="I37" s="1" t="n">
         <v>2086</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>196</v>
+        <v>243</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>197</v>
+        <v>244</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>187</v>
+        <v>231</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="G38" s="1" t="n">
+        <v>232</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="H38" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="I38" s="1" t="n">
         <v>2071</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>201</v>
+        <v>249</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>202</v>
+        <v>250</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>187</v>
+        <v>231</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="F39" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="G39" s="1" t="n">
+        <v>232</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="H39" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="I39" s="1" t="n">
         <v>2076</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>206</v>
+        <v>255</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>207</v>
+        <v>256</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>208</v>
+        <v>257</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="F40" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="G40" s="1" t="n">
+        <v>258</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="H40" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="I40" s="1" t="n">
         <v>2041</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>212</v>
+        <v>263</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>213</v>
+        <v>264</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>208</v>
+        <v>257</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="F41" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="G41" s="1" t="n">
+        <v>258</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="H41" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="I41" s="1" t="n">
         <v>2072</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>217</v>
+        <v>269</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>218</v>
+        <v>270</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>219</v>
+        <v>271</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="F42" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="G42" s="1" t="n">
+        <v>272</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="H42" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="I42" s="1" t="n">
         <v>2096</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>223</v>
+        <v>277</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>224</v>
+        <v>278</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>219</v>
+        <v>271</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="F43" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="G43" s="1" t="n">
+        <v>272</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="H43" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="I43" s="1" t="n">
         <v>2081</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>228</v>
+        <v>283</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>229</v>
+        <v>284</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>219</v>
+        <v>271</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="F44" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="G44" s="1" t="n">
+        <v>272</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="H44" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="I44" s="1" t="n">
         <v>2039</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>233</v>
+        <v>289</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>234</v>
+        <v>290</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>219</v>
+        <v>271</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="F45" s="3" t="s">
-        <v>237</v>
-      </c>
-      <c r="G45" s="1" t="n">
+        <v>272</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="H45" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="I45" s="1" t="n">
         <v>2082</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>238</v>
+        <v>295</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>239</v>
+        <v>296</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>219</v>
+        <v>271</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="F46" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="G46" s="1" t="n">
+        <v>272</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="H46" s="4" t="s">
+        <v>300</v>
+      </c>
+      <c r="I46" s="1" t="n">
         <v>2073</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>243</v>
+        <v>301</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>244</v>
+        <v>302</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>219</v>
+        <v>271</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="F47" s="3" t="s">
-        <v>247</v>
-      </c>
-      <c r="G47" s="1" t="n">
+        <v>272</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="H47" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="I47" s="1" t="n">
         <v>2084</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>248</v>
+        <v>307</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>249</v>
+        <v>308</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>219</v>
+        <v>271</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>251</v>
+        <v>272</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>309</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="G48" s="1" t="n">
+        <v>310</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="I48" s="1" t="n">
         <v>2108</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>253</v>
+        <v>313</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>254</v>
+        <v>314</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>255</v>
+        <v>315</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="F49" s="3" t="s">
-        <v>258</v>
-      </c>
-      <c r="G49" s="1" t="n">
+        <v>316</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="H49" s="4" t="s">
+        <v>320</v>
+      </c>
+      <c r="I49" s="1" t="n">
         <v>2079</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>259</v>
+        <v>321</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>260</v>
+        <v>322</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>261</v>
+        <v>323</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="F50" s="3" t="s">
-        <v>264</v>
-      </c>
-      <c r="G50" s="1" t="n">
+        <v>324</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="H50" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="I50" s="1" t="n">
         <v>2038</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>265</v>
+        <v>329</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>266</v>
+        <v>330</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>261</v>
+        <v>323</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="F51" s="3" t="s">
-        <v>269</v>
-      </c>
-      <c r="G51" s="1" t="n">
+        <v>324</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="H51" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="I51" s="1" t="n">
         <v>2102</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>270</v>
+        <v>335</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>271</v>
+        <v>336</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>261</v>
+        <v>323</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="F52" s="3" t="s">
-        <v>274</v>
-      </c>
-      <c r="G52" s="1" t="n">
+        <v>324</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="H52" s="4" t="s">
+        <v>340</v>
+      </c>
+      <c r="I52" s="1" t="n">
         <v>2027</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>275</v>
+        <v>341</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>276</v>
+        <v>342</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>261</v>
+        <v>323</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="F53" s="3" t="s">
-        <v>279</v>
-      </c>
-      <c r="G53" s="1" t="n">
+        <v>324</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="H53" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="I53" s="1" t="n">
         <v>2098</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>280</v>
+        <v>347</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>281</v>
+        <v>348</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>282</v>
+        <v>349</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="F54" s="3" t="s">
-        <v>285</v>
-      </c>
-      <c r="G54" s="1" t="n">
+        <v>350</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="H54" s="4" t="s">
+        <v>354</v>
+      </c>
+      <c r="I54" s="1" t="n">
         <v>2035</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>286</v>
+        <v>355</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>287</v>
+        <v>356</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>288</v>
+        <v>357</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="F55" s="3" t="s">
-        <v>291</v>
-      </c>
-      <c r="G55" s="1" t="n">
+        <v>358</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="H55" s="4" t="s">
+        <v>362</v>
+      </c>
+      <c r="I55" s="1" t="n">
         <v>2092</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>292</v>
+        <v>363</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>293</v>
+        <v>364</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>288</v>
+        <v>357</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>295</v>
+        <v>358</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>365</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="G56" s="1" t="n">
+        <v>366</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="I56" s="1" t="n">
         <v>2103</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>297</v>
+        <v>369</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>298</v>
+        <v>370</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>288</v>
+        <v>357</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="E57" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="F57" s="3" t="s">
-        <v>301</v>
-      </c>
-      <c r="G57" s="1" t="n">
+        <v>358</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="H57" s="4" t="s">
+        <v>374</v>
+      </c>
+      <c r="I57" s="1" t="n">
         <v>2101</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>302</v>
+        <v>375</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>303</v>
+        <v>376</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>288</v>
+        <v>357</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>305</v>
+        <v>358</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>377</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="G58" s="1" t="n">
+        <v>378</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="I58" s="1" t="n">
         <v>2106</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>307</v>
+        <v>381</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>308</v>
+        <v>382</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>288</v>
+        <v>357</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="F59" s="3" t="s">
-        <v>311</v>
-      </c>
-      <c r="G59" s="1" t="n">
+        <v>358</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="H59" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="I59" s="1" t="n">
         <v>2097</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>312</v>
+        <v>387</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>313</v>
+        <v>388</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>288</v>
+        <v>357</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="F60" s="3" t="s">
-        <v>316</v>
-      </c>
-      <c r="G60" s="1" t="n">
+        <v>358</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="H60" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="I60" s="1" t="n">
         <v>2091</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>317</v>
+        <v>393</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>318</v>
+        <v>394</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>288</v>
+        <v>357</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="F61" s="3" t="s">
-        <v>321</v>
-      </c>
-      <c r="G61" s="1" t="n">
+        <v>358</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="H61" s="4" t="s">
+        <v>398</v>
+      </c>
+      <c r="I61" s="1" t="n">
         <v>2095</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>322</v>
+        <v>399</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>323</v>
+        <v>400</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>288</v>
+        <v>357</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="F62" s="3" t="s">
-        <v>326</v>
-      </c>
-      <c r="G62" s="1" t="n">
+        <v>358</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="H62" s="4" t="s">
+        <v>404</v>
+      </c>
+      <c r="I62" s="1" t="n">
         <v>2099</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>327</v>
+        <v>405</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>328</v>
+        <v>406</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>288</v>
+        <v>357</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="F63" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="G63" s="1" t="n">
+        <v>358</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="H63" s="4" t="s">
+        <v>410</v>
+      </c>
+      <c r="I63" s="1" t="n">
         <v>2075</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>332</v>
+        <v>411</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>333</v>
+        <v>412</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>288</v>
+        <v>357</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>334</v>
-      </c>
-      <c r="E64" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="F64" s="3" t="s">
-        <v>336</v>
-      </c>
-      <c r="G64" s="1" t="n">
+        <v>358</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>413</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="H64" s="4" t="s">
+        <v>416</v>
+      </c>
+      <c r="I64" s="1" t="n">
         <v>2025</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>337</v>
+        <v>417</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>338</v>
+        <v>418</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>339</v>
+        <v>419</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="E65" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="F65" s="3" t="s">
-        <v>341</v>
-      </c>
-      <c r="G65" s="1" t="n">
+        <v>420</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>421</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="H65" s="4" t="s">
+        <v>423</v>
+      </c>
+      <c r="I65" s="1" t="n">
         <v>2051</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>342</v>
+        <v>424</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>343</v>
+        <v>425</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>339</v>
+        <v>419</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="F66" s="3" t="s">
-        <v>344</v>
-      </c>
-      <c r="G66" s="1" t="n">
+        <v>420</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>426</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="H66" s="4" t="s">
+        <v>427</v>
+      </c>
+      <c r="I66" s="1" t="n">
         <v>2052</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>345</v>
+        <v>428</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>346</v>
+        <v>429</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>339</v>
+        <v>419</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="E67" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="F67" s="3" t="s">
-        <v>347</v>
-      </c>
-      <c r="G67" s="1" t="n">
+        <v>420</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>430</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="H67" s="4" t="s">
+        <v>431</v>
+      </c>
+      <c r="I67" s="1" t="n">
         <v>2053</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>348</v>
+        <v>432</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>349</v>
+        <v>433</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>339</v>
+        <v>419</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="E68" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="F68" s="3" t="s">
-        <v>350</v>
-      </c>
-      <c r="G68" s="1" t="n">
+        <v>420</v>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>434</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="H68" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="I68" s="1" t="n">
         <v>2054</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>351</v>
+        <v>436</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>352</v>
+        <v>437</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>339</v>
+        <v>419</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="E69" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="F69" s="3" t="s">
-        <v>353</v>
-      </c>
-      <c r="G69" s="1" t="n">
+        <v>420</v>
+      </c>
+      <c r="E69" s="3" t="s">
+        <v>438</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="H69" s="4" t="s">
+        <v>439</v>
+      </c>
+      <c r="I69" s="1" t="n">
         <v>2055</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>354</v>
+        <v>440</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>355</v>
+        <v>441</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>339</v>
+        <v>419</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="E70" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="F70" s="3" t="s">
-        <v>356</v>
-      </c>
-      <c r="G70" s="1" t="n">
+        <v>420</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="H70" s="4" t="s">
+        <v>443</v>
+      </c>
+      <c r="I70" s="1" t="n">
         <v>2056</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>357</v>
+        <v>444</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>358</v>
+        <v>445</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>339</v>
+        <v>419</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="E71" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="F71" s="3" t="s">
-        <v>359</v>
-      </c>
-      <c r="G71" s="1" t="n">
+        <v>420</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>446</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="G71" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="H71" s="4" t="s">
+        <v>447</v>
+      </c>
+      <c r="I71" s="1" t="n">
         <v>2057</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>360</v>
+        <v>448</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>361</v>
+        <v>449</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>339</v>
+        <v>419</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="E72" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="F72" s="3" t="s">
-        <v>362</v>
-      </c>
-      <c r="G72" s="1" t="n">
+        <v>420</v>
+      </c>
+      <c r="E72" s="3" t="s">
+        <v>450</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="H72" s="4" t="s">
+        <v>451</v>
+      </c>
+      <c r="I72" s="1" t="n">
         <v>2058</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>363</v>
+        <v>452</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>364</v>
+        <v>453</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>339</v>
+        <v>419</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="E73" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="F73" s="3" t="s">
-        <v>365</v>
-      </c>
-      <c r="G73" s="1" t="n">
+        <v>420</v>
+      </c>
+      <c r="E73" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="G73" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="H73" s="4" t="s">
+        <v>455</v>
+      </c>
+      <c r="I73" s="1" t="n">
         <v>2059</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
-        <v>366</v>
+        <v>456</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>367</v>
+        <v>457</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>339</v>
+        <v>419</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="E74" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="F74" s="3" t="s">
-        <v>368</v>
-      </c>
-      <c r="G74" s="1" t="n">
+        <v>420</v>
+      </c>
+      <c r="E74" s="3" t="s">
+        <v>458</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="G74" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="H74" s="4" t="s">
+        <v>459</v>
+      </c>
+      <c r="I74" s="1" t="n">
         <v>2060</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
-        <v>369</v>
+        <v>460</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>370</v>
+        <v>461</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>339</v>
+        <v>419</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="E75" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="F75" s="3" t="s">
-        <v>371</v>
-      </c>
-      <c r="G75" s="1" t="n">
+        <v>420</v>
+      </c>
+      <c r="E75" s="3" t="s">
+        <v>462</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="G75" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="H75" s="4" t="s">
+        <v>463</v>
+      </c>
+      <c r="I75" s="1" t="n">
         <v>2061</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
-        <v>372</v>
+        <v>464</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>373</v>
+        <v>465</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>339</v>
+        <v>419</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="E76" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="F76" s="3" t="s">
-        <v>374</v>
-      </c>
-      <c r="G76" s="1" t="n">
+        <v>420</v>
+      </c>
+      <c r="E76" s="3" t="s">
+        <v>466</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="G76" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="H76" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="I76" s="1" t="n">
         <v>2062</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
-        <v>375</v>
+        <v>468</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>376</v>
+        <v>469</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>339</v>
+        <v>419</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="E77" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="F77" s="3" t="s">
-        <v>377</v>
-      </c>
-      <c r="G77" s="1" t="n">
+        <v>420</v>
+      </c>
+      <c r="E77" s="3" t="s">
+        <v>470</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="G77" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="H77" s="4" t="s">
+        <v>471</v>
+      </c>
+      <c r="I77" s="1" t="n">
         <v>2063</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
-        <v>378</v>
+        <v>472</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>379</v>
+        <v>473</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>339</v>
+        <v>419</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="E78" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="F78" s="3" t="s">
-        <v>380</v>
-      </c>
-      <c r="G78" s="1" t="n">
+        <v>420</v>
+      </c>
+      <c r="E78" s="3" t="s">
+        <v>474</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="G78" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="H78" s="4" t="s">
+        <v>475</v>
+      </c>
+      <c r="I78" s="1" t="n">
         <v>2064</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
-        <v>381</v>
+        <v>476</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>382</v>
+        <v>477</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>339</v>
+        <v>419</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="E79" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="F79" s="3" t="s">
-        <v>383</v>
-      </c>
-      <c r="G79" s="1" t="n">
+        <v>420</v>
+      </c>
+      <c r="E79" s="3" t="s">
+        <v>478</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="G79" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="H79" s="4" t="s">
+        <v>479</v>
+      </c>
+      <c r="I79" s="1" t="n">
         <v>2065</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
-        <v>384</v>
+        <v>480</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>385</v>
+        <v>481</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>339</v>
+        <v>419</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="E80" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="F80" s="3" t="s">
-        <v>386</v>
-      </c>
-      <c r="G80" s="1" t="n">
+        <v>420</v>
+      </c>
+      <c r="E80" s="3" t="s">
+        <v>482</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="G80" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="H80" s="4" t="s">
+        <v>483</v>
+      </c>
+      <c r="I80" s="1" t="n">
         <v>2066</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
-        <v>387</v>
+        <v>484</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>388</v>
+        <v>485</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>339</v>
+        <v>419</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="E81" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="F81" s="3" t="s">
-        <v>389</v>
-      </c>
-      <c r="G81" s="1" t="n">
+        <v>420</v>
+      </c>
+      <c r="E81" s="3" t="s">
+        <v>486</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="G81" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="H81" s="4" t="s">
+        <v>487</v>
+      </c>
+      <c r="I81" s="1" t="n">
         <v>2067</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
-        <v>390</v>
+        <v>488</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>391</v>
+        <v>489</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>339</v>
+        <v>419</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="E82" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="F82" s="3" t="s">
-        <v>392</v>
-      </c>
-      <c r="G82" s="1" t="n">
+        <v>420</v>
+      </c>
+      <c r="E82" s="3" t="s">
+        <v>490</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="G82" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="H82" s="4" t="s">
+        <v>491</v>
+      </c>
+      <c r="I82" s="1" t="n">
         <v>2068</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
-        <v>393</v>
+        <v>492</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>394</v>
+        <v>493</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>339</v>
+        <v>419</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="E83" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="F83" s="3" t="s">
-        <v>395</v>
-      </c>
-      <c r="G83" s="1" t="n">
+        <v>420</v>
+      </c>
+      <c r="E83" s="3" t="s">
+        <v>494</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="G83" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="H83" s="4" t="s">
+        <v>495</v>
+      </c>
+      <c r="I83" s="1" t="n">
         <v>2069</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="s">
-        <v>396</v>
+        <v>496</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>397</v>
+        <v>497</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>339</v>
+        <v>419</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="E84" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="F84" s="3" t="s">
-        <v>398</v>
-      </c>
-      <c r="G84" s="1" t="n">
+        <v>420</v>
+      </c>
+      <c r="E84" s="3" t="s">
+        <v>498</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="G84" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="H84" s="4" t="s">
+        <v>499</v>
+      </c>
+      <c r="I84" s="1" t="n">
         <v>2070</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="s">
-        <v>399</v>
+        <v>500</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>400</v>
+        <v>501</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>401</v>
+        <v>502</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>402</v>
-      </c>
-      <c r="E85" s="1" t="s">
-        <v>403</v>
-      </c>
-      <c r="F85" s="3" t="s">
-        <v>404</v>
-      </c>
-      <c r="G85" s="1" t="n">
+        <v>503</v>
+      </c>
+      <c r="E85" s="3" t="s">
+        <v>504</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="G85" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="H85" s="4" t="s">
+        <v>507</v>
+      </c>
+      <c r="I85" s="1" t="n">
         <v>2080</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="s">
-        <v>405</v>
+        <v>508</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>406</v>
+        <v>509</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>401</v>
+        <v>502</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>407</v>
-      </c>
-      <c r="E86" s="1" t="s">
-        <v>408</v>
-      </c>
-      <c r="F86" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="G86" s="1" t="n">
+        <v>503</v>
+      </c>
+      <c r="E86" s="3" t="s">
+        <v>510</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="G86" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="H86" s="4" t="s">
+        <v>513</v>
+      </c>
+      <c r="I86" s="1" t="n">
         <v>2085</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G86"/>
+  <autoFilter ref="A1:I86"/>
   <hyperlinks>
-    <hyperlink ref="F11" r:id="rId1" display="https://filarmonicabogota.gov.co/nosotros/proposito-objetivo-valores/"/>
-    <hyperlink ref="F13" r:id="rId2" display="https://es.investinbogota.org/quienes-somos/"/>
-    <hyperlink ref="F33" r:id="rId3" display="https://etb.com/corporativo/UploadFile/Calificaciones_Informes/Resultados-2T2016-ETB.pdf"/>
-    <hyperlink ref="F48" r:id="rId4" display="https://www.umv.gov.co/portal/quienes-somos-2/"/>
-    <hyperlink ref="F56" r:id="rId5" display="https://bogota.gov.co/mi-ciudad/salud/bogota-bio-produccion-de-vacunas-para-el-pais-en-plan-de-desarrollo"/>
-    <hyperlink ref="F58" r:id="rId6" display="https://bogota.gov.co/mi-ciudad/salud/que-es-el-fondo-financiero-distrital-de-salud-secretaria-de-salud"/>
+    <hyperlink ref="H11" r:id="rId1" display="https://filarmonicabogota.gov.co/nosotros/proposito-objetivo-valores/"/>
+    <hyperlink ref="H13" r:id="rId2" display="https://es.investinbogota.org/quienes-somos/"/>
+    <hyperlink ref="H33" r:id="rId3" display="https://etb.com/corporativo/UploadFile/Calificaciones_Informes/Resultados-2T2016-ETB.pdf"/>
+    <hyperlink ref="H48" r:id="rId4" display="https://www.umv.gov.co/portal/quienes-somos-2/"/>
+    <hyperlink ref="H56" r:id="rId5" display="https://bogota.gov.co/mi-ciudad/salud/bogota-bio-produccion-de-vacunas-para-el-pais-en-plan-de-desarrollo"/>
+    <hyperlink ref="H58" r:id="rId6" display="https://bogota.gov.co/mi-ciudad/salud/que-es-el-fondo-financiero-distrital-de-salud-secretaria-de-salud"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>